<commit_message>
after outfall samples pulled
</commit_message>
<xml_diff>
--- a/LakeHodges/Equipment Settings - Storm 1.xlsx
+++ b/LakeHodges/Equipment Settings - Storm 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sutron" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="199">
   <si>
     <t>SD900 Sampler Settings</t>
   </si>
@@ -410,9 +410,6 @@
     <t>sampling_on (1= ON, 0=OFF)</t>
   </si>
   <si>
-    <t>2.0 in</t>
-  </si>
-  <si>
     <t>4.5 in</t>
   </si>
   <si>
@@ -539,9 +536,6 @@
     <t>If Velocity is being recorded</t>
   </si>
   <si>
-    <t>1.0 in</t>
-  </si>
-  <si>
     <t>9.5 in</t>
   </si>
   <si>
@@ -615,6 +609,21 @@
   </si>
   <si>
     <t>0,3.0,0,3.85</t>
+  </si>
+  <si>
+    <t>1.0 in &gt;&gt;&gt; 0.1in</t>
+  </si>
+  <si>
+    <t>65000 &gt;&gt;&gt; 100</t>
+  </si>
+  <si>
+    <t>13000 &gt;&gt;&gt; 25</t>
+  </si>
+  <si>
+    <t>2.0 in &gt;&gt;&gt; 0.2 in</t>
+  </si>
+  <si>
+    <t>15000 &gt;&gt;&gt; 900</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1201,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1283,7 +1292,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1291,7 +1300,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1299,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1307,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1346,10 +1355,10 @@
         <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1375,10 +1384,10 @@
         <v>40</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1404,10 +1413,10 @@
         <v>40</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1433,10 +1442,10 @@
         <v>40</v>
       </c>
       <c r="H14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1449,8 +1458,8 @@
       <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="23">
-        <v>65000</v>
+      <c r="D15" s="23" t="s">
+        <v>195</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -1462,10 +1471,10 @@
         <v>40</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1478,8 +1487,8 @@
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="23">
-        <v>15000</v>
+      <c r="D16" s="23" t="s">
+        <v>198</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1491,10 +1500,10 @@
         <v>40</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>127</v>
+        <v>197</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1507,8 +1516,8 @@
       <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="23">
-        <v>13000</v>
+      <c r="D17" s="23" t="s">
+        <v>196</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1520,10 +1529,10 @@
         <v>40</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1549,10 +1558,10 @@
         <v>40</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1578,10 +1587,10 @@
         <v>40</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1593,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1644,7 +1653,7 @@
       </c>
       <c r="S1" s="1"/>
       <c r="Z1" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AA1" s="17"/>
       <c r="AB1" s="18"/>
@@ -1699,7 +1708,7 @@
         <v>89</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>91</v>
@@ -1726,13 +1735,13 @@
         <v>97</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AA2" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB2" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AB2" s="21" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
@@ -1975,13 +1984,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7">
         <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E7" t="s">
         <v>74</v>
@@ -1996,7 +2005,7 @@
         <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J7" t="s">
         <v>123</v>
@@ -2044,7 +2053,7 @@
         <v>98</v>
       </c>
       <c r="Z7" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA7" s="9">
         <v>0.25</v>
@@ -2058,13 +2067,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8">
         <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" t="s">
         <v>74</v>
@@ -2076,10 +2085,10 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I8" t="s">
         <v>146</v>
-      </c>
-      <c r="I8" t="s">
-        <v>147</v>
       </c>
       <c r="J8" t="s">
         <v>80</v>
@@ -2127,7 +2136,7 @@
         <v>98</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA8" s="9">
         <v>0</v>
@@ -2157,13 +2166,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" t="s">
         <v>74</v>
@@ -2172,10 +2181,10 @@
         <v>119</v>
       </c>
       <c r="G10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>152</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>153</v>
       </c>
       <c r="J10" t="s">
         <v>123</v>
@@ -2208,7 +2217,7 @@
         <v>125</v>
       </c>
       <c r="U10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V10" t="s">
         <v>125</v>
@@ -2220,7 +2229,7 @@
         <v>98</v>
       </c>
       <c r="Z10" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
@@ -2228,7 +2237,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2243,10 +2252,10 @@
         <v>119</v>
       </c>
       <c r="G11" t="s">
+        <v>159</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>161</v>
       </c>
       <c r="J11" t="s">
         <v>123</v>
@@ -2279,7 +2288,7 @@
         <v>125</v>
       </c>
       <c r="U11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V11" t="s">
         <v>125</v>
@@ -2291,7 +2300,7 @@
         <v>98</v>
       </c>
       <c r="Z11" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
@@ -2299,13 +2308,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" t="s">
         <v>74</v>
@@ -2314,10 +2323,10 @@
         <v>119</v>
       </c>
       <c r="G12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J12" t="s">
         <v>123</v>
@@ -2353,7 +2362,7 @@
         <v>125</v>
       </c>
       <c r="U12" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V12" s="15" t="s">
         <v>125</v>
@@ -2365,7 +2374,7 @@
         <v>98</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
@@ -2373,10 +2382,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E13" t="s">
         <v>74</v>
@@ -2385,10 +2394,10 @@
         <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J13" t="s">
         <v>123</v>
@@ -2421,7 +2430,7 @@
         <v>125</v>
       </c>
       <c r="U13" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V13" s="15" t="s">
         <v>125</v>
@@ -2433,13 +2442,13 @@
         <v>98</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA13" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AB13" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
@@ -2447,7 +2456,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2459,13 +2468,13 @@
         <v>74</v>
       </c>
       <c r="F14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G14" t="s">
+        <v>188</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>189</v>
-      </c>
-      <c r="G14" t="s">
-        <v>190</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>191</v>
       </c>
       <c r="J14" t="s">
         <v>123</v>
@@ -2498,7 +2507,7 @@
         <v>125</v>
       </c>
       <c r="U14" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V14" s="15" t="s">
         <v>125</v>
@@ -2510,13 +2519,13 @@
         <v>98</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA14" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AB14" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
@@ -2524,7 +2533,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2536,13 +2545,13 @@
         <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J15" t="s">
         <v>123</v>
@@ -2573,7 +2582,7 @@
         <v>125</v>
       </c>
       <c r="U15" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V15" s="15" t="s">
         <v>125</v>
@@ -2585,13 +2594,13 @@
         <v>98</v>
       </c>
       <c r="Z15" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA15" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AB15" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
@@ -2599,7 +2608,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -2608,13 +2617,13 @@
         <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J16" t="s">
         <v>123</v>
@@ -2659,13 +2668,13 @@
         <v>98</v>
       </c>
       <c r="Z16" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA16" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AB16" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -2673,13 +2682,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E17" t="s">
         <v>74</v>
@@ -2694,7 +2703,7 @@
         <v>36</v>
       </c>
       <c r="I17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J17" t="s">
         <v>123</v>
@@ -2736,7 +2745,7 @@
         <v>98</v>
       </c>
       <c r="Z17" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -2808,7 +2817,7 @@
         <v>98</v>
       </c>
       <c r="Z18" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
@@ -2917,11 +2926,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD16"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3196,10 +3205,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -3235,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q7" t="s">
         <v>64</v>
@@ -3258,7 +3267,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>
@@ -3294,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q8" t="s">
         <v>64</v>
@@ -3319,10 +3328,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" t="s">
         <v>45</v>
@@ -3358,7 +3367,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q10" t="s">
         <v>64</v>
@@ -3381,7 +3390,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E11" t="s">
         <v>45</v>
@@ -3440,7 +3449,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
         <v>45</v>
@@ -3476,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q12" t="s">
         <v>64</v>
@@ -3499,7 +3508,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
@@ -3511,7 +3520,7 @@
         <v>46</v>
       </c>
       <c r="H13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I13" t="s">
         <v>23</v>
@@ -3520,22 +3529,22 @@
         <v>51</v>
       </c>
       <c r="K13" t="s">
+        <v>174</v>
+      </c>
+      <c r="L13" t="s">
+        <v>175</v>
+      </c>
+      <c r="M13" t="s">
         <v>176</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
         <v>177</v>
-      </c>
-      <c r="M13" t="s">
-        <v>178</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>179</v>
       </c>
       <c r="Q13" t="s">
         <v>64</v>
@@ -3558,7 +3567,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
@@ -3567,7 +3576,7 @@
         <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H14" t="s">
         <v>110</v>
@@ -3585,7 +3594,7 @@
         <v>55</v>
       </c>
       <c r="M14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -3617,7 +3626,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E15" t="s">
         <v>45</v>
@@ -3644,7 +3653,7 @@
         <v>55</v>
       </c>
       <c r="M15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -3653,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q15" t="s">
         <v>64</v>
@@ -3676,7 +3685,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E16" t="s">
         <v>45</v>
@@ -3703,7 +3712,7 @@
         <v>55</v>
       </c>
       <c r="M16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -3712,7 +3721,7 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Q16" t="s">
         <v>64</v>
@@ -3735,7 +3744,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>

</xml_diff>